<commit_message>
registration page related checkin
</commit_message>
<xml_diff>
--- a/testData/NewPython.xlsx
+++ b/testData/NewPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheet\git\Testng_DSalgo\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BCBC88-790E-40B7-97C5-1C367D237A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23E9F9B-A9E1-4CFC-84CB-CB84D65B84B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{310D9AC9-EA90-49EA-95DD-C5373C8C659A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>code</t>
   </si>
@@ -77,6 +77,27 @@
   </si>
   <si>
     <t>Element Not Found</t>
+  </si>
+  <si>
+    <t>ninja4!</t>
+  </si>
+  <si>
+    <t>abcd123@</t>
+  </si>
+  <si>
+    <t>ninja4</t>
+  </si>
+  <si>
+    <t>abcd123</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>confirmPassword</t>
   </si>
 </sst>
 </file>
@@ -177,12 +198,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -550,39 +569,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE76D5B-3C13-4E69-8EDF-0DFC89667648}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17" style="7" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="22" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="7"/>
+    <col min="1" max="1" width="17" style="6" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="22" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="5"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="5"/>
-    </row>
-    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
@@ -592,7 +635,7 @@
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
-      <c r="C6" s="8"/>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
@@ -608,11 +651,6 @@
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>